<commit_message>
feat: added yearly repeated measures
</commit_message>
<xml_diff>
--- a/dictionaries/example-dictionary/example-dictionary-yearly_rep.xlsx
+++ b/dictionaries/example-dictionary/example-dictionary-yearly_rep.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/VisualStudioCodeProjects/ds-beta-dictionaries/dictionaries/example-dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{432A4ABB-BA65-064A-AE6C-F458D24B3892}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFAB0CB8-B9CF-0E46-80A7-AAF54BE5408E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="75900" yWindow="2260" windowWidth="15960" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,9 +50,6 @@
     <t>Unique identifier of the child_id</t>
   </si>
   <si>
-    <t>integer</t>
-  </si>
-  <si>
     <t>age_years</t>
   </si>
   <si>
@@ -60,6 +57,9 @@
   </si>
   <si>
     <t>Height of the child</t>
+  </si>
+  <si>
+    <t>decimal</t>
   </si>
 </sst>
 </file>
@@ -1289,7 +1289,7 @@
   <dimension ref="A1:IP4"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1575,7 +1575,7 @@
     </row>
     <row r="3" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -1589,16 +1589,16 @@
     </row>
     <row r="4" spans="1:250" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>